<commit_message>
Updated_realizing in Bootstrap that divided by 360 is not necessary as we are taking year as time unit
</commit_message>
<xml_diff>
--- a/xlsx/hw4.xlsx
+++ b/xlsx/hw4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13466\source\repos\xll_ml\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1E5E62-921A-41ED-9685-6BE459BC6654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D59CA276-EBE8-4A77-89B4-10A5DC3379F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3108" yWindow="1332" windowWidth="19176" windowHeight="12480" activeTab="1" xr2:uid="{EDEE3299-5466-402C-8B4F-6E69C4CA67FB}"/>
+    <workbookView xWindow="3396" yWindow="2088" windowWidth="19176" windowHeight="12480" activeTab="3" xr2:uid="{EDEE3299-5466-402C-8B4F-6E69C4CA67FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Treasury Rates" sheetId="1" r:id="rId1"/>
@@ -758,211 +758,211 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="69"/>
                 <c:pt idx="0">
-                  <c:v>1.0313874368449654E-4</c:v>
+                  <c:v>3.715831656820115E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.035142317659301E-4</c:v>
+                  <c:v>3.7323037168694624E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0319536825936958E-4</c:v>
+                  <c:v>3.7294240837115154E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0277943042752876E-4</c:v>
+                  <c:v>3.721079054557859E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0138994732094902E-4</c:v>
+                  <c:v>3.6778519999290514E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0000018246136307E-4</c:v>
+                  <c:v>3.632691013270551E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.8982943136249161E-5</c:v>
+                  <c:v>3.6059207069266165E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.8256343618310661E-5</c:v>
+                  <c:v>3.5867990595380914E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.7711393979856768E-5</c:v>
+                  <c:v>3.5724578239966977E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.7287544261059322E-5</c:v>
+                  <c:v>3.5613035296867254E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.6948464486021349E-5</c:v>
+                  <c:v>3.5523800942387468E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.3173759772428536E-2</c:v>
+                  <c:v>3.4565988638108697E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.4712165426399794E-2</c:v>
+                  <c:v>3.4087082485969311E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.477437710056816E-2</c:v>
+                  <c:v>3.4271966353096553E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.4815851550013738E-2</c:v>
+                  <c:v>3.4395222264514712E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.5344223875980733E-2</c:v>
+                  <c:v>3.4979007110321814E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.5740503120455978E-2</c:v>
+                  <c:v>3.5416845744677142E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.604872031060339E-2</c:v>
+                  <c:v>3.5757386904731278E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.6295294062721327E-2</c:v>
+                  <c:v>3.6029819832774604E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.6945179466388506E-2</c:v>
+                  <c:v>3.6699769586277319E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.7486750636111149E-2</c:v>
+                  <c:v>3.725806104752958E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3.7945003164338006E-2</c:v>
+                  <c:v>3.7730461514743033E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.8337791045675314E-2</c:v>
+                  <c:v>3.8135376200925997E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.8882386521731156E-2</c:v>
+                  <c:v>3.8690866617754754E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.9358907563280018E-2</c:v>
+                  <c:v>3.9176920732479914E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.9779367305823134E-2</c:v>
+                  <c:v>3.9605792010178588E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4.0153109299194786E-2</c:v>
+                  <c:v>3.9987010923688518E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.0487510030106269E-2</c:v>
+                  <c:v>4.0328101530513194E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>4.0788470687926605E-2</c:v>
+                  <c:v>4.06350830766554E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4.1426325230369251E-2</c:v>
+                  <c:v>4.1278260592309116E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>4.200619299622621E-2</c:v>
+                  <c:v>4.1862967424721592E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>4.2535637478095606E-2</c:v>
+                  <c:v>4.2396830184750371E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4.3020961586475885E-2</c:v>
+                  <c:v>4.2886204381443416E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>4.346745976618574E-2</c:v>
+                  <c:v>4.3336428642401031E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>4.3879611932071759E-2</c:v>
+                  <c:v>4.3752020267900343E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4.4261234307892146E-2</c:v>
+                  <c:v>4.413682732854788E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4.4615597942582512E-2</c:v>
+                  <c:v>4.4494148170577723E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4.4945522705914918E-2</c:v>
+                  <c:v>4.4826826195915853E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4.5253452485025165E-2</c:v>
+                  <c:v>4.5137325686231439E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4.5541515826773453E-2</c:v>
+                  <c:v>4.5427792951365377E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4.5811575209662482E-2</c:v>
+                  <c:v>4.5700106012428444E-2</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>4.6065267357224902E-2</c:v>
+                  <c:v>4.59559152516089E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4.6304036437283647E-2</c:v>
+                  <c:v>4.6196676888484632E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>4.6529161569910465E-2</c:v>
+                  <c:v>4.6423680717538877E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>4.6741779750724681E-2</c:v>
+                  <c:v>4.6638073222756787E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>4.694290505690029E-2</c:v>
+                  <c:v>4.6840876943908857E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>4.7133444820645611E-2</c:v>
+                  <c:v>4.7033006785000303E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>4.7314213314455268E-2</c:v>
+                  <c:v>4.7215283813728075E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>4.7485943383574439E-2</c:v>
+                  <c:v>4.7388446991019462E-2</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>4.7511833371737464E-2</c:v>
+                  <c:v>4.7416517109592764E-2</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>4.7536490503321288E-2</c:v>
+                  <c:v>4.744325055585305E-2</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>4.756000079157563E-2</c:v>
+                  <c:v>4.746874058600821E-2</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>4.7582442430363872E-2</c:v>
+                  <c:v>4.7493071978429044E-2</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>4.7603886662983749E-2</c:v>
+                  <c:v>4.7516321975631173E-2</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>4.7624398537663627E-2</c:v>
+                  <c:v>4.7538561103389727E-2</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>4.7644037566612452E-2</c:v>
+                  <c:v>4.7559853885286218E-2</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>4.7662858302688405E-2</c:v>
+                  <c:v>4.7580259467937029E-2</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>4.7680910845455136E-2</c:v>
+                  <c:v>4.7599832169663313E-2</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>4.7698241286511199E-2</c:v>
+                  <c:v>4.7618621963320534E-2</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>4.7714892102427804E-2</c:v>
+                  <c:v>4.7636674902324545E-2</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>4.773090250234762E-2</c:v>
+                  <c:v>4.7654033497520704E-2</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>4.7746308736232722E-2</c:v>
+                  <c:v>4.767073705138871E-2</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>4.7761144368862835E-2</c:v>
+                  <c:v>4.7686821955113451E-2</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>4.7775440523942739E-2</c:v>
+                  <c:v>4.7702321953248202E-2</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>4.7789226102055514E-2</c:v>
+                  <c:v>4.7717268380021001E-2</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>4.7802527975673109E-2</c:v>
+                  <c:v>4.7731690370766675E-2</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>4.7815371163993543E-2</c:v>
+                  <c:v>4.7745615051486646E-2</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>4.7827778989998029E-2</c:v>
+                  <c:v>4.7759067709131367E-2</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>4.7839773221802363E-2</c:v>
+                  <c:v>4.777207194485459E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1235,211 +1235,211 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="69"/>
                 <c:pt idx="0">
-                  <c:v>1.0313874368449654E-4</c:v>
+                  <c:v>3.715831656820115E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0539167217309795E-4</c:v>
+                  <c:v>3.814664017116199E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.011128615701034E-4</c:v>
+                  <c:v>3.6683596176462913E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0278224795759079E-4</c:v>
+                  <c:v>3.7404183748547974E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.4441123023019248E-5</c:v>
+                  <c:v>3.4520470666365488E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.4441123023019248E-5</c:v>
+                  <c:v>3.4520470666365488E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.3896746510679631E-5</c:v>
+                  <c:v>3.4720691752069432E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.3896746510679631E-5</c:v>
+                  <c:v>3.4720691752069432E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.3896746510679631E-5</c:v>
+                  <c:v>3.4720691752069432E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.3896746510679631E-5</c:v>
+                  <c:v>3.4720691752069432E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.3896746510679631E-5</c:v>
+                  <c:v>3.4720691752069432E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.9327382388313569E-2</c:v>
+                  <c:v>3.2650364029551147E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.9327382388313569E-2</c:v>
+                  <c:v>3.2650364029551147E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.5023223797241633E-2</c:v>
+                  <c:v>3.5011501821605513E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.5023223797241633E-2</c:v>
+                  <c:v>3.5011501821605513E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.8514457831782707E-2</c:v>
+                  <c:v>3.8481716185164432E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.8514457831782707E-2</c:v>
+                  <c:v>3.8481716185164432E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.8514457831782707E-2</c:v>
+                  <c:v>3.8481716185164432E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.8514457831782707E-2</c:v>
+                  <c:v>3.8481716185164432E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.3444033503060267E-2</c:v>
+                  <c:v>4.3399267121304493E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.3444033503060267E-2</c:v>
+                  <c:v>4.3399267121304493E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4.3444033503060267E-2</c:v>
+                  <c:v>4.3399267121304493E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4.3444033503060267E-2</c:v>
+                  <c:v>4.3399267121304493E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4.6506723186512944E-2</c:v>
+                  <c:v>4.6467732453357329E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4.6506723186512944E-2</c:v>
+                  <c:v>4.6467732453357329E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4.6506723186512944E-2</c:v>
+                  <c:v>4.6467732453357329E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4.6506723186512944E-2</c:v>
+                  <c:v>4.6467732453357329E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.6506723186512944E-2</c:v>
+                  <c:v>4.6467732453357329E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>4.6506723186512944E-2</c:v>
+                  <c:v>4.6467732453357329E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>5.418341607922228E-2</c:v>
+                  <c:v>5.4141810905383524E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>5.418341607922228E-2</c:v>
+                  <c:v>5.4141810905383524E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>5.418341607922228E-2</c:v>
+                  <c:v>5.4141810905383524E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>5.418341607922228E-2</c:v>
+                  <c:v>5.4141810905383524E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>5.418341607922228E-2</c:v>
+                  <c:v>5.4141810905383524E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>5.418341607922228E-2</c:v>
+                  <c:v>5.4141810905383524E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>5.418341607922228E-2</c:v>
+                  <c:v>5.4141810905383524E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>5.418341607922228E-2</c:v>
+                  <c:v>5.4141810905383524E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>5.418341607922228E-2</c:v>
+                  <c:v>5.4141810905383524E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>5.418341607922228E-2</c:v>
+                  <c:v>5.4141810905383524E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>5.418341607922228E-2</c:v>
+                  <c:v>5.4141810905383524E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>5.418341607922228E-2</c:v>
+                  <c:v>5.4141810905383524E-2</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>5.418341607922228E-2</c:v>
+                  <c:v>5.4141810905383524E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>5.418341607922228E-2</c:v>
+                  <c:v>5.4141810905383524E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>5.418341607922228E-2</c:v>
+                  <c:v>5.4141810905383524E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>5.418341607922228E-2</c:v>
+                  <c:v>5.4141810905383524E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>5.418341607922228E-2</c:v>
+                  <c:v>5.4141810905383524E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>5.418341607922228E-2</c:v>
+                  <c:v>5.4141810905383524E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>5.418341607922228E-2</c:v>
+                  <c:v>5.4141810905383524E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>5.418341607922228E-2</c:v>
+                  <c:v>5.4141810905383524E-2</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>4.8547432898258212E-2</c:v>
+                  <c:v>4.8539321852524846E-2</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>4.8547432898258212E-2</c:v>
+                  <c:v>4.8539321852524846E-2</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>4.8547432898258212E-2</c:v>
+                  <c:v>4.8539321852524846E-2</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>4.8547432898258212E-2</c:v>
+                  <c:v>4.8539321852524846E-2</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>4.8547432898258212E-2</c:v>
+                  <c:v>4.8539321852524846E-2</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>4.8547432898258212E-2</c:v>
+                  <c:v>4.8539321852524846E-2</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>4.8547432898258212E-2</c:v>
+                  <c:v>4.8539321852524846E-2</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>4.8547432898258212E-2</c:v>
+                  <c:v>4.8539321852524846E-2</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>4.8547432898258212E-2</c:v>
+                  <c:v>4.8539321852524846E-2</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>4.8547432898258212E-2</c:v>
+                  <c:v>4.8539321852524846E-2</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>4.8547432898258212E-2</c:v>
+                  <c:v>4.8539321852524846E-2</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>4.8547432898258212E-2</c:v>
+                  <c:v>4.8539321852524846E-2</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>4.8547432898258212E-2</c:v>
+                  <c:v>4.8539321852524846E-2</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>4.8547432898258212E-2</c:v>
+                  <c:v>4.8539321852524846E-2</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>4.8547432898258212E-2</c:v>
+                  <c:v>4.8539321852524846E-2</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>4.8547432898258212E-2</c:v>
+                  <c:v>4.8539321852524846E-2</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>4.8547432898258212E-2</c:v>
+                  <c:v>4.8539321852524846E-2</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>4.8547432898258212E-2</c:v>
+                  <c:v>4.8539321852524846E-2</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>4.8547432898258212E-2</c:v>
+                  <c:v>4.8539321852524846E-2</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>4.8547432898258212E-2</c:v>
+                  <c:v>4.8539321852524846E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4191,8 +4191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{674E2F35-77D5-4361-8DFB-2603DE31162A}">
   <dimension ref="A2:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -4245,7 +4245,7 @@
       <c r="A5" s="8"/>
       <c r="B5" s="11" cm="1">
         <f t="array" ref="B5">_xll.\FI.INSTRUMENT(B3:E3,B4:E4)</f>
-        <v>2108863780496</v>
+        <v>2139811972544</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>33</v>
@@ -4313,7 +4313,7 @@
       <c r="A10" s="8"/>
       <c r="B10" s="12" cm="1">
         <f t="array" ref="B10">_xll.\FI.INSTRUMENT.ZERO_COUPON_BOND(B8,B9)</f>
-        <v>2110523736064</v>
+        <v>2139811973120</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>34</v>
@@ -4349,7 +4349,7 @@
       </c>
       <c r="B13" s="12" cm="1">
         <f t="array" ref="B13">_xll.\FI.INSTRUMENT.BOND(2,0.5,2)</f>
-        <v>2110732027264</v>
+        <v>2139912826208</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>35</v>
@@ -4454,7 +4454,7 @@
     <row r="5" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B5" cm="1">
         <f t="array" ref="B5">_xll.\FI.CURVE.PWFLAT(B3:E3,B4:E4)</f>
-        <v>2110908399376</v>
+        <v>2139811976864</v>
       </c>
       <c r="C5" t="s">
         <v>31</v>
@@ -4503,15 +4503,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF2E5B4B-30B9-4C78-A319-DEE69FDAA7AA}">
   <dimension ref="B2:T75"/>
   <sheetViews>
-    <sheetView zoomScale="89" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="4" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.08203125" customWidth="1"/>
-    <col min="6" max="15" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="15" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="10.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.35">
@@ -4535,7 +4537,7 @@
       </c>
       <c r="I2" cm="1">
         <f t="array" ref="I2">_xll.\FI.CURVE.PWFLAT.BOOTSTRAP(_xlfn.ANCHORARRAY(G3),_xlfn.ANCHORARRAY(G4))</f>
-        <v>2110728488496</v>
+        <v>2139811979168</v>
       </c>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.35">
@@ -4550,55 +4552,55 @@
         <v>3.7100000000000001E-2</v>
       </c>
       <c r="E3">
-        <f>1-D3*C3/360</f>
-        <v>0.99999141203703701</v>
+        <f>1-D3*C3</f>
+        <v>0.99690833333333329</v>
       </c>
       <c r="F3" s="6" cm="1">
         <f t="array" ref="F3">_xll.\FI.INSTRUMENT.ZERO_COUPON_BOND(C3)</f>
-        <v>2110728483888</v>
+        <v>2139811973984</v>
       </c>
       <c r="G3" cm="1">
         <f t="array" ref="G3:T3">TRANSPOSE(F3:F16)</f>
-        <v>2110728483888</v>
+        <v>2139811973984</v>
       </c>
       <c r="H3">
-        <v>2110908422272</v>
+        <v>2139811974416</v>
       </c>
       <c r="I3">
-        <v>2110908422848</v>
+        <v>2139811977440</v>
       </c>
       <c r="J3">
-        <v>2110908419824</v>
+        <v>2139811975856</v>
       </c>
       <c r="K3">
-        <v>2110908414352</v>
+        <v>2139811974992</v>
       </c>
       <c r="L3">
-        <v>2110908410608</v>
+        <v>2139811977152</v>
       </c>
       <c r="M3">
-        <v>2110908406288</v>
+        <v>2139811976000</v>
       </c>
       <c r="N3">
-        <v>2110905579056</v>
+        <v>2139912825888</v>
       </c>
       <c r="O3">
-        <v>2110905581936</v>
+        <v>2139912821728</v>
       </c>
       <c r="P3">
-        <v>2110905581776</v>
+        <v>2139912819968</v>
       </c>
       <c r="Q3">
-        <v>2110905575696</v>
+        <v>2139905529344</v>
       </c>
       <c r="R3">
-        <v>2110905575536</v>
+        <v>2139905528544</v>
       </c>
       <c r="S3">
-        <v>2110905583216</v>
+        <v>2139910659584</v>
       </c>
       <c r="T3">
-        <v>2110905588176</v>
+        <v>2139912823808</v>
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.35">
@@ -4613,34 +4615,34 @@
         <v>3.7400000000000003E-2</v>
       </c>
       <c r="E4">
-        <f>1-D4*C4/360</f>
-        <v>0.99998701388888889</v>
+        <f t="shared" ref="E4:E9" si="0">1-D4*C4</f>
+        <v>0.99532500000000002</v>
       </c>
       <c r="F4" cm="1">
         <f t="array" ref="F4">_xll.\FI.INSTRUMENT.ZERO_COUPON_BOND(C4)</f>
-        <v>2110908422272</v>
+        <v>2139811974416</v>
       </c>
       <c r="G4" cm="1">
         <f t="array" ref="G4:T4">TRANSPOSE(E3:E16)</f>
-        <v>0.99999141203703701</v>
+        <v>0.99690833333333329</v>
       </c>
       <c r="H4">
-        <v>0.99998701388888889</v>
+        <v>0.99532500000000002</v>
       </c>
       <c r="I4">
-        <v>0.99998273148148153</v>
+        <v>0.99378333333333335</v>
       </c>
       <c r="J4">
-        <v>0.99997430555555555</v>
+        <v>0.99075000000000002</v>
       </c>
       <c r="K4">
-        <v>0.99996574074074074</v>
+        <v>0.98766666666666669</v>
       </c>
       <c r="L4">
-        <v>0.99995000000000001</v>
+        <v>0.98199999999999998</v>
       </c>
       <c r="M4">
-        <v>0.99990305555555559</v>
+        <v>0.96509999999999996</v>
       </c>
       <c r="N4">
         <v>1</v>
@@ -4676,12 +4678,12 @@
         <v>3.73E-2</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:E9" si="0">1-D5*C5/360</f>
-        <v>0.99998273148148153</v>
+        <f t="shared" si="0"/>
+        <v>0.99378333333333335</v>
       </c>
       <c r="F5" cm="1">
         <f t="array" ref="F5">_xll.\FI.INSTRUMENT.ZERO_COUPON_BOND(C5)</f>
-        <v>2110908422848</v>
+        <v>2139811977440</v>
       </c>
       <c r="I5" t="s">
         <v>27</v>
@@ -4700,11 +4702,11 @@
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>0.99997430555555555</v>
+        <v>0.99075000000000002</v>
       </c>
       <c r="F6" cm="1">
         <f t="array" ref="F6">_xll.\FI.INSTRUMENT.ZERO_COUPON_BOND(C6)</f>
-        <v>2110908419824</v>
+        <v>2139811975856</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>23</v>
@@ -4729,11 +4731,11 @@
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>0.99996574074074074</v>
+        <v>0.98766666666666669</v>
       </c>
       <c r="F7" cm="1">
         <f t="array" ref="F7">_xll.\FI.INSTRUMENT.ZERO_COUPON_BOND(C7)</f>
-        <v>2110908414352</v>
+        <v>2139811974992</v>
       </c>
       <c r="H7">
         <v>0.1</v>
@@ -4744,11 +4746,11 @@
       </c>
       <c r="J7" cm="1">
         <f t="array" ref="J7">_xll.FI.CURVE.SPOT($I$2,I7)</f>
-        <v>1.0313874368449654E-4</v>
+        <v>3.715831656820115E-2</v>
       </c>
       <c r="K7" cm="1">
         <f t="array" ref="K7">_xll.FI.CURVE.FORWARD($I$2,I7)</f>
-        <v>1.0313874368449654E-4</v>
+        <v>3.715831656820115E-2</v>
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.35">
@@ -4764,11 +4766,11 @@
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>0.99995000000000001</v>
+        <v>0.98199999999999998</v>
       </c>
       <c r="F8" cm="1">
         <f t="array" ref="F8">_xll.\FI.INSTRUMENT.ZERO_COUPON_BOND(C8)</f>
-        <v>2110908410608</v>
+        <v>2139811977152</v>
       </c>
       <c r="H8">
         <v>0.5</v>
@@ -4778,11 +4780,11 @@
       </c>
       <c r="J8" cm="1">
         <f t="array" ref="J8">_xll.FI.CURVE.SPOT($I$2,I8)</f>
-        <v>1.035142317659301E-4</v>
+        <v>3.7323037168694624E-2</v>
       </c>
       <c r="K8" cm="1">
         <f t="array" ref="K8">_xll.FI.CURVE.FORWARD($I$2,I8)</f>
-        <v>1.0539167217309795E-4</v>
+        <v>3.814664017116199E-2</v>
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.35">
@@ -4797,22 +4799,22 @@
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>0.99990305555555559</v>
+        <v>0.96509999999999996</v>
       </c>
       <c r="F9" cm="1">
         <f t="array" ref="F9">_xll.\FI.INSTRUMENT.ZERO_COUPON_BOND(C9)</f>
-        <v>2110908406288</v>
+        <v>2139811976000</v>
       </c>
       <c r="I9">
         <v>0.2</v>
       </c>
       <c r="J9" cm="1">
         <f t="array" ref="J9">_xll.FI.CURVE.SPOT($I$2,I9)</f>
-        <v>1.0319536825936958E-4</v>
+        <v>3.7294240837115154E-2</v>
       </c>
       <c r="K9" cm="1">
         <f t="array" ref="K9">_xll.FI.CURVE.FORWARD($I$2,I9)</f>
-        <v>1.011128615701034E-4</v>
+        <v>3.6683596176462913E-2</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.35">
@@ -4830,18 +4832,18 @@
       </c>
       <c r="F10" s="6" cm="1">
         <f t="array" ref="F10">_xll.\FI.INSTRUMENT.BOND(C10,D10,1)</f>
-        <v>2110905579056</v>
+        <v>2139912825888</v>
       </c>
       <c r="I10">
         <v>0.30000000000000004</v>
       </c>
       <c r="J10" cm="1">
         <f t="array" ref="J10">_xll.FI.CURVE.SPOT($I$2,I10)</f>
-        <v>1.0277943042752876E-4</v>
+        <v>3.721079054557859E-2</v>
       </c>
       <c r="K10" cm="1">
         <f t="array" ref="K10">_xll.FI.CURVE.FORWARD($I$2,I10)</f>
-        <v>1.0278224795759079E-4</v>
+        <v>3.7404183748547974E-2</v>
       </c>
       <c r="L10" s="6" t="s">
         <v>26</v>
@@ -4862,18 +4864,18 @@
       </c>
       <c r="F11" cm="1">
         <f t="array" ref="F11">_xll.\FI.INSTRUMENT.BOND(C11,D11,1)</f>
-        <v>2110905581936</v>
+        <v>2139912821728</v>
       </c>
       <c r="I11">
         <v>0.4</v>
       </c>
       <c r="J11" cm="1">
         <f t="array" ref="J11">_xll.FI.CURVE.SPOT($I$2,I11)</f>
-        <v>1.0138994732094902E-4</v>
+        <v>3.6778519999290514E-2</v>
       </c>
       <c r="K11" cm="1">
         <f t="array" ref="K11">_xll.FI.CURVE.FORWARD($I$2,I11)</f>
-        <v>9.4441123023019248E-5</v>
+        <v>3.4520470666365488E-2</v>
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.35">
@@ -4891,18 +4893,18 @@
       </c>
       <c r="F12" cm="1">
         <f t="array" ref="F12">_xll.\FI.INSTRUMENT.BOND(C12,D12,1)</f>
-        <v>2110905581776</v>
+        <v>2139912819968</v>
       </c>
       <c r="I12">
         <v>0.5</v>
       </c>
       <c r="J12" cm="1">
         <f t="array" ref="J12">_xll.FI.CURVE.SPOT($I$2,I12)</f>
-        <v>1.0000018246136307E-4</v>
+        <v>3.632691013270551E-2</v>
       </c>
       <c r="K12" cm="1">
         <f t="array" ref="K12">_xll.FI.CURVE.FORWARD($I$2,I12)</f>
-        <v>9.4441123023019248E-5</v>
+        <v>3.4520470666365488E-2</v>
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.35">
@@ -4920,18 +4922,18 @@
       </c>
       <c r="F13" cm="1">
         <f t="array" ref="F13">_xll.\FI.INSTRUMENT.BOND(C13,D13,1)</f>
-        <v>2110905575696</v>
+        <v>2139905529344</v>
       </c>
       <c r="I13">
         <v>0.6</v>
       </c>
       <c r="J13" cm="1">
         <f t="array" ref="J13">_xll.FI.CURVE.SPOT($I$2,I13)</f>
-        <v>9.8982943136249161E-5</v>
+        <v>3.6059207069266165E-2</v>
       </c>
       <c r="K13" cm="1">
         <f t="array" ref="K13">_xll.FI.CURVE.FORWARD($I$2,I13)</f>
-        <v>9.3896746510679631E-5</v>
+        <v>3.4720691752069432E-2</v>
       </c>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.35">
@@ -4949,18 +4951,18 @@
       </c>
       <c r="F14" cm="1">
         <f t="array" ref="F14">_xll.\FI.INSTRUMENT.BOND(C14,D14,1)</f>
-        <v>2110905575536</v>
+        <v>2139905528544</v>
       </c>
       <c r="I14">
         <v>0.7</v>
       </c>
       <c r="J14" cm="1">
         <f t="array" ref="J14">_xll.FI.CURVE.SPOT($I$2,I14)</f>
-        <v>9.8256343618310661E-5</v>
+        <v>3.5867990595380914E-2</v>
       </c>
       <c r="K14" cm="1">
         <f t="array" ref="K14">_xll.FI.CURVE.FORWARD($I$2,I14)</f>
-        <v>9.3896746510679631E-5</v>
+        <v>3.4720691752069432E-2</v>
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.35">
@@ -4978,18 +4980,18 @@
       </c>
       <c r="F15" cm="1">
         <f t="array" ref="F15">_xll.\FI.INSTRUMENT.BOND(C15,D15,1)</f>
-        <v>2110905583216</v>
+        <v>2139910659584</v>
       </c>
       <c r="I15">
         <v>0.79999999999999993</v>
       </c>
       <c r="J15" cm="1">
         <f t="array" ref="J15">_xll.FI.CURVE.SPOT($I$2,I15)</f>
-        <v>9.7711393979856768E-5</v>
+        <v>3.5724578239966977E-2</v>
       </c>
       <c r="K15" cm="1">
         <f t="array" ref="K15">_xll.FI.CURVE.FORWARD($I$2,I15)</f>
-        <v>9.3896746510679631E-5</v>
+        <v>3.4720691752069432E-2</v>
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.35">
@@ -5007,18 +5009,18 @@
       </c>
       <c r="F16" cm="1">
         <f t="array" ref="F16">_xll.\FI.INSTRUMENT.BOND(C16,D16,1)</f>
-        <v>2110905588176</v>
+        <v>2139912823808</v>
       </c>
       <c r="I16">
         <v>0.89999999999999991</v>
       </c>
       <c r="J16" cm="1">
         <f t="array" ref="J16">_xll.FI.CURVE.SPOT($I$2,I16)</f>
-        <v>9.7287544261059322E-5</v>
+        <v>3.5613035296867254E-2</v>
       </c>
       <c r="K16" cm="1">
         <f t="array" ref="K16">_xll.FI.CURVE.FORWARD($I$2,I16)</f>
-        <v>9.3896746510679631E-5</v>
+        <v>3.4720691752069432E-2</v>
       </c>
     </row>
     <row r="17" spans="9:11" x14ac:dyDescent="0.35">
@@ -5027,11 +5029,11 @@
       </c>
       <c r="J17" cm="1">
         <f t="array" ref="J17">_xll.FI.CURVE.SPOT($I$2,I17)</f>
-        <v>9.6948464486021349E-5</v>
+        <v>3.5523800942387468E-2</v>
       </c>
       <c r="K17" cm="1">
         <f t="array" ref="K17">_xll.FI.CURVE.FORWARD($I$2,I17)</f>
-        <v>9.3896746510679631E-5</v>
+        <v>3.4720691752069432E-2</v>
       </c>
     </row>
     <row r="18" spans="9:11" x14ac:dyDescent="0.35">
@@ -5040,11 +5042,11 @@
       </c>
       <c r="J18" cm="1">
         <f t="array" ref="J18">_xll.FI.CURVE.SPOT($I$2,I18)</f>
-        <v>2.3173759772428536E-2</v>
+        <v>3.4565988638108697E-2</v>
       </c>
       <c r="K18" cm="1">
         <f t="array" ref="K18">_xll.FI.CURVE.FORWARD($I$2,I18)</f>
-        <v>6.9327382388313569E-2</v>
+        <v>3.2650364029551147E-2</v>
       </c>
     </row>
     <row r="19" spans="9:11" x14ac:dyDescent="0.35">
@@ -5053,11 +5055,11 @@
       </c>
       <c r="J19" cm="1">
         <f t="array" ref="J19">_xll.FI.CURVE.SPOT($I$2,I19)</f>
-        <v>3.4712165426399794E-2</v>
+        <v>3.4087082485969311E-2</v>
       </c>
       <c r="K19" cm="1">
         <f t="array" ref="K19">_xll.FI.CURVE.FORWARD($I$2,I19)</f>
-        <v>6.9327382388313569E-2</v>
+        <v>3.2650364029551147E-2</v>
       </c>
     </row>
     <row r="20" spans="9:11" x14ac:dyDescent="0.35">
@@ -5066,11 +5068,11 @@
       </c>
       <c r="J20" cm="1">
         <f t="array" ref="J20">_xll.FI.CURVE.SPOT($I$2,I20)</f>
-        <v>3.477437710056816E-2</v>
+        <v>3.4271966353096553E-2</v>
       </c>
       <c r="K20" cm="1">
         <f t="array" ref="K20">_xll.FI.CURVE.FORWARD($I$2,I20)</f>
-        <v>3.5023223797241633E-2</v>
+        <v>3.5011501821605513E-2</v>
       </c>
     </row>
     <row r="21" spans="9:11" x14ac:dyDescent="0.35">
@@ -5079,11 +5081,11 @@
       </c>
       <c r="J21" cm="1">
         <f t="array" ref="J21">_xll.FI.CURVE.SPOT($I$2,I21)</f>
-        <v>3.4815851550013738E-2</v>
+        <v>3.4395222264514712E-2</v>
       </c>
       <c r="K21" cm="1">
         <f t="array" ref="K21">_xll.FI.CURVE.FORWARD($I$2,I21)</f>
-        <v>3.5023223797241633E-2</v>
+        <v>3.5011501821605513E-2</v>
       </c>
     </row>
     <row r="22" spans="9:11" x14ac:dyDescent="0.35">
@@ -5092,11 +5094,11 @@
       </c>
       <c r="J22" cm="1">
         <f t="array" ref="J22">_xll.FI.CURVE.SPOT($I$2,I22)</f>
-        <v>3.5344223875980733E-2</v>
+        <v>3.4979007110321814E-2</v>
       </c>
       <c r="K22" cm="1">
         <f t="array" ref="K22">_xll.FI.CURVE.FORWARD($I$2,I22)</f>
-        <v>3.8514457831782707E-2</v>
+        <v>3.8481716185164432E-2</v>
       </c>
     </row>
     <row r="23" spans="9:11" x14ac:dyDescent="0.35">
@@ -5105,11 +5107,11 @@
       </c>
       <c r="J23" cm="1">
         <f t="array" ref="J23">_xll.FI.CURVE.SPOT($I$2,I23)</f>
-        <v>3.5740503120455978E-2</v>
+        <v>3.5416845744677142E-2</v>
       </c>
       <c r="K23" cm="1">
         <f t="array" ref="K23">_xll.FI.CURVE.FORWARD($I$2,I23)</f>
-        <v>3.8514457831782707E-2</v>
+        <v>3.8481716185164432E-2</v>
       </c>
     </row>
     <row r="24" spans="9:11" x14ac:dyDescent="0.35">
@@ -5118,11 +5120,11 @@
       </c>
       <c r="J24" cm="1">
         <f t="array" ref="J24">_xll.FI.CURVE.SPOT($I$2,I24)</f>
-        <v>3.604872031060339E-2</v>
+        <v>3.5757386904731278E-2</v>
       </c>
       <c r="K24" cm="1">
         <f t="array" ref="K24">_xll.FI.CURVE.FORWARD($I$2,I24)</f>
-        <v>3.8514457831782707E-2</v>
+        <v>3.8481716185164432E-2</v>
       </c>
     </row>
     <row r="25" spans="9:11" x14ac:dyDescent="0.35">
@@ -5131,11 +5133,11 @@
       </c>
       <c r="J25" cm="1">
         <f t="array" ref="J25">_xll.FI.CURVE.SPOT($I$2,I25)</f>
-        <v>3.6295294062721327E-2</v>
+        <v>3.6029819832774604E-2</v>
       </c>
       <c r="K25" cm="1">
         <f t="array" ref="K25">_xll.FI.CURVE.FORWARD($I$2,I25)</f>
-        <v>3.8514457831782707E-2</v>
+        <v>3.8481716185164432E-2</v>
       </c>
     </row>
     <row r="26" spans="9:11" x14ac:dyDescent="0.35">
@@ -5144,11 +5146,11 @@
       </c>
       <c r="J26" cm="1">
         <f t="array" ref="J26">_xll.FI.CURVE.SPOT($I$2,I26)</f>
-        <v>3.6945179466388506E-2</v>
+        <v>3.6699769586277319E-2</v>
       </c>
       <c r="K26" cm="1">
         <f t="array" ref="K26">_xll.FI.CURVE.FORWARD($I$2,I26)</f>
-        <v>4.3444033503060267E-2</v>
+        <v>4.3399267121304493E-2</v>
       </c>
     </row>
     <row r="27" spans="9:11" x14ac:dyDescent="0.35">
@@ -5157,11 +5159,11 @@
       </c>
       <c r="J27" cm="1">
         <f t="array" ref="J27">_xll.FI.CURVE.SPOT($I$2,I27)</f>
-        <v>3.7486750636111149E-2</v>
+        <v>3.725806104752958E-2</v>
       </c>
       <c r="K27" cm="1">
         <f t="array" ref="K27">_xll.FI.CURVE.FORWARD($I$2,I27)</f>
-        <v>4.3444033503060267E-2</v>
+        <v>4.3399267121304493E-2</v>
       </c>
     </row>
     <row r="28" spans="9:11" x14ac:dyDescent="0.35">
@@ -5170,11 +5172,11 @@
       </c>
       <c r="J28" cm="1">
         <f t="array" ref="J28">_xll.FI.CURVE.SPOT($I$2,I28)</f>
-        <v>3.7945003164338006E-2</v>
+        <v>3.7730461514743033E-2</v>
       </c>
       <c r="K28" cm="1">
         <f t="array" ref="K28">_xll.FI.CURVE.FORWARD($I$2,I28)</f>
-        <v>4.3444033503060267E-2</v>
+        <v>4.3399267121304493E-2</v>
       </c>
     </row>
     <row r="29" spans="9:11" x14ac:dyDescent="0.35">
@@ -5183,11 +5185,11 @@
       </c>
       <c r="J29" cm="1">
         <f t="array" ref="J29">_xll.FI.CURVE.SPOT($I$2,I29)</f>
-        <v>3.8337791045675314E-2</v>
+        <v>3.8135376200925997E-2</v>
       </c>
       <c r="K29" cm="1">
         <f t="array" ref="K29">_xll.FI.CURVE.FORWARD($I$2,I29)</f>
-        <v>4.3444033503060267E-2</v>
+        <v>4.3399267121304493E-2</v>
       </c>
     </row>
     <row r="30" spans="9:11" x14ac:dyDescent="0.35">
@@ -5196,11 +5198,11 @@
       </c>
       <c r="J30" cm="1">
         <f t="array" ref="J30">_xll.FI.CURVE.SPOT($I$2,I30)</f>
-        <v>3.8882386521731156E-2</v>
+        <v>3.8690866617754754E-2</v>
       </c>
       <c r="K30" cm="1">
         <f t="array" ref="K30">_xll.FI.CURVE.FORWARD($I$2,I30)</f>
-        <v>4.6506723186512944E-2</v>
+        <v>4.6467732453357329E-2</v>
       </c>
     </row>
     <row r="31" spans="9:11" x14ac:dyDescent="0.35">
@@ -5209,11 +5211,11 @@
       </c>
       <c r="J31" cm="1">
         <f t="array" ref="J31">_xll.FI.CURVE.SPOT($I$2,I31)</f>
-        <v>3.9358907563280018E-2</v>
+        <v>3.9176920732479914E-2</v>
       </c>
       <c r="K31" cm="1">
         <f t="array" ref="K31">_xll.FI.CURVE.FORWARD($I$2,I31)</f>
-        <v>4.6506723186512944E-2</v>
+        <v>4.6467732453357329E-2</v>
       </c>
     </row>
     <row r="32" spans="9:11" x14ac:dyDescent="0.35">
@@ -5222,11 +5224,11 @@
       </c>
       <c r="J32" cm="1">
         <f t="array" ref="J32">_xll.FI.CURVE.SPOT($I$2,I32)</f>
-        <v>3.9779367305823134E-2</v>
+        <v>3.9605792010178588E-2</v>
       </c>
       <c r="K32" cm="1">
         <f t="array" ref="K32">_xll.FI.CURVE.FORWARD($I$2,I32)</f>
-        <v>4.6506723186512944E-2</v>
+        <v>4.6467732453357329E-2</v>
       </c>
     </row>
     <row r="33" spans="9:11" x14ac:dyDescent="0.35">
@@ -5235,11 +5237,11 @@
       </c>
       <c r="J33" cm="1">
         <f t="array" ref="J33">_xll.FI.CURVE.SPOT($I$2,I33)</f>
-        <v>4.0153109299194786E-2</v>
+        <v>3.9987010923688518E-2</v>
       </c>
       <c r="K33" cm="1">
         <f t="array" ref="K33">_xll.FI.CURVE.FORWARD($I$2,I33)</f>
-        <v>4.6506723186512944E-2</v>
+        <v>4.6467732453357329E-2</v>
       </c>
     </row>
     <row r="34" spans="9:11" x14ac:dyDescent="0.35">
@@ -5248,11 +5250,11 @@
       </c>
       <c r="J34" cm="1">
         <f t="array" ref="J34">_xll.FI.CURVE.SPOT($I$2,I34)</f>
-        <v>4.0487510030106269E-2</v>
+        <v>4.0328101530513194E-2</v>
       </c>
       <c r="K34" cm="1">
         <f t="array" ref="K34">_xll.FI.CURVE.FORWARD($I$2,I34)</f>
-        <v>4.6506723186512944E-2</v>
+        <v>4.6467732453357329E-2</v>
       </c>
     </row>
     <row r="35" spans="9:11" x14ac:dyDescent="0.35">
@@ -5261,11 +5263,11 @@
       </c>
       <c r="J35" cm="1">
         <f t="array" ref="J35">_xll.FI.CURVE.SPOT($I$2,I35)</f>
-        <v>4.0788470687926605E-2</v>
+        <v>4.06350830766554E-2</v>
       </c>
       <c r="K35" cm="1">
         <f t="array" ref="K35">_xll.FI.CURVE.FORWARD($I$2,I35)</f>
-        <v>4.6506723186512944E-2</v>
+        <v>4.6467732453357329E-2</v>
       </c>
     </row>
     <row r="36" spans="9:11" x14ac:dyDescent="0.35">
@@ -5274,11 +5276,11 @@
       </c>
       <c r="J36" cm="1">
         <f t="array" ref="J36">_xll.FI.CURVE.SPOT($I$2,I36)</f>
-        <v>4.1426325230369251E-2</v>
+        <v>4.1278260592309116E-2</v>
       </c>
       <c r="K36" cm="1">
         <f t="array" ref="K36">_xll.FI.CURVE.FORWARD($I$2,I36)</f>
-        <v>5.418341607922228E-2</v>
+        <v>5.4141810905383524E-2</v>
       </c>
     </row>
     <row r="37" spans="9:11" x14ac:dyDescent="0.35">
@@ -5287,11 +5289,11 @@
       </c>
       <c r="J37" cm="1">
         <f t="array" ref="J37">_xll.FI.CURVE.SPOT($I$2,I37)</f>
-        <v>4.200619299622621E-2</v>
+        <v>4.1862967424721592E-2</v>
       </c>
       <c r="K37" cm="1">
         <f t="array" ref="K37">_xll.FI.CURVE.FORWARD($I$2,I37)</f>
-        <v>5.418341607922228E-2</v>
+        <v>5.4141810905383524E-2</v>
       </c>
     </row>
     <row r="38" spans="9:11" x14ac:dyDescent="0.35">
@@ -5300,11 +5302,11 @@
       </c>
       <c r="J38" cm="1">
         <f t="array" ref="J38">_xll.FI.CURVE.SPOT($I$2,I38)</f>
-        <v>4.2535637478095606E-2</v>
+        <v>4.2396830184750371E-2</v>
       </c>
       <c r="K38" cm="1">
         <f t="array" ref="K38">_xll.FI.CURVE.FORWARD($I$2,I38)</f>
-        <v>5.418341607922228E-2</v>
+        <v>5.4141810905383524E-2</v>
       </c>
     </row>
     <row r="39" spans="9:11" x14ac:dyDescent="0.35">
@@ -5313,11 +5315,11 @@
       </c>
       <c r="J39" cm="1">
         <f t="array" ref="J39">_xll.FI.CURVE.SPOT($I$2,I39)</f>
-        <v>4.3020961586475885E-2</v>
+        <v>4.2886204381443416E-2</v>
       </c>
       <c r="K39" cm="1">
         <f t="array" ref="K39">_xll.FI.CURVE.FORWARD($I$2,I39)</f>
-        <v>5.418341607922228E-2</v>
+        <v>5.4141810905383524E-2</v>
       </c>
     </row>
     <row r="40" spans="9:11" x14ac:dyDescent="0.35">
@@ -5326,11 +5328,11 @@
       </c>
       <c r="J40" cm="1">
         <f t="array" ref="J40">_xll.FI.CURVE.SPOT($I$2,I40)</f>
-        <v>4.346745976618574E-2</v>
+        <v>4.3336428642401031E-2</v>
       </c>
       <c r="K40" cm="1">
         <f t="array" ref="K40">_xll.FI.CURVE.FORWARD($I$2,I40)</f>
-        <v>5.418341607922228E-2</v>
+        <v>5.4141810905383524E-2</v>
       </c>
     </row>
     <row r="41" spans="9:11" x14ac:dyDescent="0.35">
@@ -5339,11 +5341,11 @@
       </c>
       <c r="J41" cm="1">
         <f t="array" ref="J41">_xll.FI.CURVE.SPOT($I$2,I41)</f>
-        <v>4.3879611932071759E-2</v>
+        <v>4.3752020267900343E-2</v>
       </c>
       <c r="K41" cm="1">
         <f t="array" ref="K41">_xll.FI.CURVE.FORWARD($I$2,I41)</f>
-        <v>5.418341607922228E-2</v>
+        <v>5.4141810905383524E-2</v>
       </c>
     </row>
     <row r="42" spans="9:11" x14ac:dyDescent="0.35">
@@ -5352,11 +5354,11 @@
       </c>
       <c r="J42" cm="1">
         <f t="array" ref="J42">_xll.FI.CURVE.SPOT($I$2,I42)</f>
-        <v>4.4261234307892146E-2</v>
+        <v>4.413682732854788E-2</v>
       </c>
       <c r="K42" cm="1">
         <f t="array" ref="K42">_xll.FI.CURVE.FORWARD($I$2,I42)</f>
-        <v>5.418341607922228E-2</v>
+        <v>5.4141810905383524E-2</v>
       </c>
     </row>
     <row r="43" spans="9:11" x14ac:dyDescent="0.35">
@@ -5365,11 +5367,11 @@
       </c>
       <c r="J43" cm="1">
         <f t="array" ref="J43">_xll.FI.CURVE.SPOT($I$2,I43)</f>
-        <v>4.4615597942582512E-2</v>
+        <v>4.4494148170577723E-2</v>
       </c>
       <c r="K43" cm="1">
         <f t="array" ref="K43">_xll.FI.CURVE.FORWARD($I$2,I43)</f>
-        <v>5.418341607922228E-2</v>
+        <v>5.4141810905383524E-2</v>
       </c>
     </row>
     <row r="44" spans="9:11" x14ac:dyDescent="0.35">
@@ -5378,11 +5380,11 @@
       </c>
       <c r="J44" cm="1">
         <f t="array" ref="J44">_xll.FI.CURVE.SPOT($I$2,I44)</f>
-        <v>4.4945522705914918E-2</v>
+        <v>4.4826826195915853E-2</v>
       </c>
       <c r="K44" cm="1">
         <f t="array" ref="K44">_xll.FI.CURVE.FORWARD($I$2,I44)</f>
-        <v>5.418341607922228E-2</v>
+        <v>5.4141810905383524E-2</v>
       </c>
     </row>
     <row r="45" spans="9:11" x14ac:dyDescent="0.35">
@@ -5391,11 +5393,11 @@
       </c>
       <c r="J45" cm="1">
         <f t="array" ref="J45">_xll.FI.CURVE.SPOT($I$2,I45)</f>
-        <v>4.5253452485025165E-2</v>
+        <v>4.5137325686231439E-2</v>
       </c>
       <c r="K45" cm="1">
         <f t="array" ref="K45">_xll.FI.CURVE.FORWARD($I$2,I45)</f>
-        <v>5.418341607922228E-2</v>
+        <v>5.4141810905383524E-2</v>
       </c>
     </row>
     <row r="46" spans="9:11" x14ac:dyDescent="0.35">
@@ -5404,11 +5406,11 @@
       </c>
       <c r="J46" cm="1">
         <f t="array" ref="J46">_xll.FI.CURVE.SPOT($I$2,I46)</f>
-        <v>4.5541515826773453E-2</v>
+        <v>4.5427792951365377E-2</v>
       </c>
       <c r="K46" cm="1">
         <f t="array" ref="K46">_xll.FI.CURVE.FORWARD($I$2,I46)</f>
-        <v>5.418341607922228E-2</v>
+        <v>5.4141810905383524E-2</v>
       </c>
     </row>
     <row r="47" spans="9:11" x14ac:dyDescent="0.35">
@@ -5417,11 +5419,11 @@
       </c>
       <c r="J47" cm="1">
         <f t="array" ref="J47">_xll.FI.CURVE.SPOT($I$2,I47)</f>
-        <v>4.5811575209662482E-2</v>
+        <v>4.5700106012428444E-2</v>
       </c>
       <c r="K47" cm="1">
         <f t="array" ref="K47">_xll.FI.CURVE.FORWARD($I$2,I47)</f>
-        <v>5.418341607922228E-2</v>
+        <v>5.4141810905383524E-2</v>
       </c>
     </row>
     <row r="48" spans="9:11" x14ac:dyDescent="0.35">
@@ -5430,11 +5432,11 @@
       </c>
       <c r="J48" cm="1">
         <f t="array" ref="J48">_xll.FI.CURVE.SPOT($I$2,I48)</f>
-        <v>4.6065267357224902E-2</v>
+        <v>4.59559152516089E-2</v>
       </c>
       <c r="K48" cm="1">
         <f t="array" ref="K48">_xll.FI.CURVE.FORWARD($I$2,I48)</f>
-        <v>5.418341607922228E-2</v>
+        <v>5.4141810905383524E-2</v>
       </c>
     </row>
     <row r="49" spans="9:11" x14ac:dyDescent="0.35">
@@ -5443,11 +5445,11 @@
       </c>
       <c r="J49" cm="1">
         <f t="array" ref="J49">_xll.FI.CURVE.SPOT($I$2,I49)</f>
-        <v>4.6304036437283647E-2</v>
+        <v>4.6196676888484632E-2</v>
       </c>
       <c r="K49" cm="1">
         <f t="array" ref="K49">_xll.FI.CURVE.FORWARD($I$2,I49)</f>
-        <v>5.418341607922228E-2</v>
+        <v>5.4141810905383524E-2</v>
       </c>
     </row>
     <row r="50" spans="9:11" x14ac:dyDescent="0.35">
@@ -5456,11 +5458,11 @@
       </c>
       <c r="J50" cm="1">
         <f t="array" ref="J50">_xll.FI.CURVE.SPOT($I$2,I50)</f>
-        <v>4.6529161569910465E-2</v>
+        <v>4.6423680717538877E-2</v>
       </c>
       <c r="K50" cm="1">
         <f t="array" ref="K50">_xll.FI.CURVE.FORWARD($I$2,I50)</f>
-        <v>5.418341607922228E-2</v>
+        <v>5.4141810905383524E-2</v>
       </c>
     </row>
     <row r="51" spans="9:11" x14ac:dyDescent="0.35">
@@ -5469,11 +5471,11 @@
       </c>
       <c r="J51" cm="1">
         <f t="array" ref="J51">_xll.FI.CURVE.SPOT($I$2,I51)</f>
-        <v>4.6741779750724681E-2</v>
+        <v>4.6638073222756787E-2</v>
       </c>
       <c r="K51" cm="1">
         <f t="array" ref="K51">_xll.FI.CURVE.FORWARD($I$2,I51)</f>
-        <v>5.418341607922228E-2</v>
+        <v>5.4141810905383524E-2</v>
       </c>
     </row>
     <row r="52" spans="9:11" x14ac:dyDescent="0.35">
@@ -5482,11 +5484,11 @@
       </c>
       <c r="J52" cm="1">
         <f t="array" ref="J52">_xll.FI.CURVE.SPOT($I$2,I52)</f>
-        <v>4.694290505690029E-2</v>
+        <v>4.6840876943908857E-2</v>
       </c>
       <c r="K52" cm="1">
         <f t="array" ref="K52">_xll.FI.CURVE.FORWARD($I$2,I52)</f>
-        <v>5.418341607922228E-2</v>
+        <v>5.4141810905383524E-2</v>
       </c>
     </row>
     <row r="53" spans="9:11" x14ac:dyDescent="0.35">
@@ -5495,11 +5497,11 @@
       </c>
       <c r="J53" cm="1">
         <f t="array" ref="J53">_xll.FI.CURVE.SPOT($I$2,I53)</f>
-        <v>4.7133444820645611E-2</v>
+        <v>4.7033006785000303E-2</v>
       </c>
       <c r="K53" cm="1">
         <f t="array" ref="K53">_xll.FI.CURVE.FORWARD($I$2,I53)</f>
-        <v>5.418341607922228E-2</v>
+        <v>5.4141810905383524E-2</v>
       </c>
     </row>
     <row r="54" spans="9:11" x14ac:dyDescent="0.35">
@@ -5508,11 +5510,11 @@
       </c>
       <c r="J54" cm="1">
         <f t="array" ref="J54">_xll.FI.CURVE.SPOT($I$2,I54)</f>
-        <v>4.7314213314455268E-2</v>
+        <v>4.7215283813728075E-2</v>
       </c>
       <c r="K54" cm="1">
         <f t="array" ref="K54">_xll.FI.CURVE.FORWARD($I$2,I54)</f>
-        <v>5.418341607922228E-2</v>
+        <v>5.4141810905383524E-2</v>
       </c>
     </row>
     <row r="55" spans="9:11" x14ac:dyDescent="0.35">
@@ -5521,11 +5523,11 @@
       </c>
       <c r="J55" cm="1">
         <f t="array" ref="J55">_xll.FI.CURVE.SPOT($I$2,I55)</f>
-        <v>4.7485943383574439E-2</v>
+        <v>4.7388446991019462E-2</v>
       </c>
       <c r="K55" cm="1">
         <f t="array" ref="K55">_xll.FI.CURVE.FORWARD($I$2,I55)</f>
-        <v>5.418341607922228E-2</v>
+        <v>5.4141810905383524E-2</v>
       </c>
     </row>
     <row r="56" spans="9:11" x14ac:dyDescent="0.35">
@@ -5534,11 +5536,11 @@
       </c>
       <c r="J56" cm="1">
         <f t="array" ref="J56">_xll.FI.CURVE.SPOT($I$2,I56)</f>
-        <v>4.7511833371737464E-2</v>
+        <v>4.7416517109592764E-2</v>
       </c>
       <c r="K56" cm="1">
         <f t="array" ref="K56">_xll.FI.CURVE.FORWARD($I$2,I56)</f>
-        <v>4.8547432898258212E-2</v>
+        <v>4.8539321852524846E-2</v>
       </c>
     </row>
     <row r="57" spans="9:11" x14ac:dyDescent="0.35">
@@ -5547,11 +5549,11 @@
       </c>
       <c r="J57" cm="1">
         <f t="array" ref="J57">_xll.FI.CURVE.SPOT($I$2,I57)</f>
-        <v>4.7536490503321288E-2</v>
+        <v>4.744325055585305E-2</v>
       </c>
       <c r="K57" cm="1">
         <f t="array" ref="K57">_xll.FI.CURVE.FORWARD($I$2,I57)</f>
-        <v>4.8547432898258212E-2</v>
+        <v>4.8539321852524846E-2</v>
       </c>
     </row>
     <row r="58" spans="9:11" x14ac:dyDescent="0.35">
@@ -5560,11 +5562,11 @@
       </c>
       <c r="J58" cm="1">
         <f t="array" ref="J58">_xll.FI.CURVE.SPOT($I$2,I58)</f>
-        <v>4.756000079157563E-2</v>
+        <v>4.746874058600821E-2</v>
       </c>
       <c r="K58" cm="1">
         <f t="array" ref="K58">_xll.FI.CURVE.FORWARD($I$2,I58)</f>
-        <v>4.8547432898258212E-2</v>
+        <v>4.8539321852524846E-2</v>
       </c>
     </row>
     <row r="59" spans="9:11" x14ac:dyDescent="0.35">
@@ -5573,11 +5575,11 @@
       </c>
       <c r="J59" cm="1">
         <f t="array" ref="J59">_xll.FI.CURVE.SPOT($I$2,I59)</f>
-        <v>4.7582442430363872E-2</v>
+        <v>4.7493071978429044E-2</v>
       </c>
       <c r="K59" cm="1">
         <f t="array" ref="K59">_xll.FI.CURVE.FORWARD($I$2,I59)</f>
-        <v>4.8547432898258212E-2</v>
+        <v>4.8539321852524846E-2</v>
       </c>
     </row>
     <row r="60" spans="9:11" x14ac:dyDescent="0.35">
@@ -5586,11 +5588,11 @@
       </c>
       <c r="J60" cm="1">
         <f t="array" ref="J60">_xll.FI.CURVE.SPOT($I$2,I60)</f>
-        <v>4.7603886662983749E-2</v>
+        <v>4.7516321975631173E-2</v>
       </c>
       <c r="K60" cm="1">
         <f t="array" ref="K60">_xll.FI.CURVE.FORWARD($I$2,I60)</f>
-        <v>4.8547432898258212E-2</v>
+        <v>4.8539321852524846E-2</v>
       </c>
     </row>
     <row r="61" spans="9:11" x14ac:dyDescent="0.35">
@@ -5599,11 +5601,11 @@
       </c>
       <c r="J61" cm="1">
         <f t="array" ref="J61">_xll.FI.CURVE.SPOT($I$2,I61)</f>
-        <v>4.7624398537663627E-2</v>
+        <v>4.7538561103389727E-2</v>
       </c>
       <c r="K61" cm="1">
         <f t="array" ref="K61">_xll.FI.CURVE.FORWARD($I$2,I61)</f>
-        <v>4.8547432898258212E-2</v>
+        <v>4.8539321852524846E-2</v>
       </c>
     </row>
     <row r="62" spans="9:11" x14ac:dyDescent="0.35">
@@ -5612,11 +5614,11 @@
       </c>
       <c r="J62" cm="1">
         <f t="array" ref="J62">_xll.FI.CURVE.SPOT($I$2,I62)</f>
-        <v>4.7644037566612452E-2</v>
+        <v>4.7559853885286218E-2</v>
       </c>
       <c r="K62" cm="1">
         <f t="array" ref="K62">_xll.FI.CURVE.FORWARD($I$2,I62)</f>
-        <v>4.8547432898258212E-2</v>
+        <v>4.8539321852524846E-2</v>
       </c>
     </row>
     <row r="63" spans="9:11" x14ac:dyDescent="0.35">
@@ -5625,11 +5627,11 @@
       </c>
       <c r="J63" cm="1">
         <f t="array" ref="J63">_xll.FI.CURVE.SPOT($I$2,I63)</f>
-        <v>4.7662858302688405E-2</v>
+        <v>4.7580259467937029E-2</v>
       </c>
       <c r="K63" cm="1">
         <f t="array" ref="K63">_xll.FI.CURVE.FORWARD($I$2,I63)</f>
-        <v>4.8547432898258212E-2</v>
+        <v>4.8539321852524846E-2</v>
       </c>
     </row>
     <row r="64" spans="9:11" x14ac:dyDescent="0.35">
@@ -5638,11 +5640,11 @@
       </c>
       <c r="J64" cm="1">
         <f t="array" ref="J64">_xll.FI.CURVE.SPOT($I$2,I64)</f>
-        <v>4.7680910845455136E-2</v>
+        <v>4.7599832169663313E-2</v>
       </c>
       <c r="K64" cm="1">
         <f t="array" ref="K64">_xll.FI.CURVE.FORWARD($I$2,I64)</f>
-        <v>4.8547432898258212E-2</v>
+        <v>4.8539321852524846E-2</v>
       </c>
     </row>
     <row r="65" spans="9:11" x14ac:dyDescent="0.35">
@@ -5651,11 +5653,11 @@
       </c>
       <c r="J65" cm="1">
         <f t="array" ref="J65">_xll.FI.CURVE.SPOT($I$2,I65)</f>
-        <v>4.7698241286511199E-2</v>
+        <v>4.7618621963320534E-2</v>
       </c>
       <c r="K65" cm="1">
         <f t="array" ref="K65">_xll.FI.CURVE.FORWARD($I$2,I65)</f>
-        <v>4.8547432898258212E-2</v>
+        <v>4.8539321852524846E-2</v>
       </c>
     </row>
     <row r="66" spans="9:11" x14ac:dyDescent="0.35">
@@ -5664,11 +5666,11 @@
       </c>
       <c r="J66" cm="1">
         <f t="array" ref="J66">_xll.FI.CURVE.SPOT($I$2,I66)</f>
-        <v>4.7714892102427804E-2</v>
+        <v>4.7636674902324545E-2</v>
       </c>
       <c r="K66" cm="1">
         <f t="array" ref="K66">_xll.FI.CURVE.FORWARD($I$2,I66)</f>
-        <v>4.8547432898258212E-2</v>
+        <v>4.8539321852524846E-2</v>
       </c>
     </row>
     <row r="67" spans="9:11" x14ac:dyDescent="0.35">
@@ -5677,11 +5679,11 @@
       </c>
       <c r="J67" cm="1">
         <f t="array" ref="J67">_xll.FI.CURVE.SPOT($I$2,I67)</f>
-        <v>4.773090250234762E-2</v>
+        <v>4.7654033497520704E-2</v>
       </c>
       <c r="K67" cm="1">
         <f t="array" ref="K67">_xll.FI.CURVE.FORWARD($I$2,I67)</f>
-        <v>4.8547432898258212E-2</v>
+        <v>4.8539321852524846E-2</v>
       </c>
     </row>
     <row r="68" spans="9:11" x14ac:dyDescent="0.35">
@@ -5690,11 +5692,11 @@
       </c>
       <c r="J68" cm="1">
         <f t="array" ref="J68">_xll.FI.CURVE.SPOT($I$2,I68)</f>
-        <v>4.7746308736232722E-2</v>
+        <v>4.767073705138871E-2</v>
       </c>
       <c r="K68" cm="1">
         <f t="array" ref="K68">_xll.FI.CURVE.FORWARD($I$2,I68)</f>
-        <v>4.8547432898258212E-2</v>
+        <v>4.8539321852524846E-2</v>
       </c>
     </row>
     <row r="69" spans="9:11" x14ac:dyDescent="0.35">
@@ -5703,11 +5705,11 @@
       </c>
       <c r="J69" cm="1">
         <f t="array" ref="J69">_xll.FI.CURVE.SPOT($I$2,I69)</f>
-        <v>4.7761144368862835E-2</v>
+        <v>4.7686821955113451E-2</v>
       </c>
       <c r="K69" cm="1">
         <f t="array" ref="K69">_xll.FI.CURVE.FORWARD($I$2,I69)</f>
-        <v>4.8547432898258212E-2</v>
+        <v>4.8539321852524846E-2</v>
       </c>
     </row>
     <row r="70" spans="9:11" x14ac:dyDescent="0.35">
@@ -5716,11 +5718,11 @@
       </c>
       <c r="J70" cm="1">
         <f t="array" ref="J70">_xll.FI.CURVE.SPOT($I$2,I70)</f>
-        <v>4.7775440523942739E-2</v>
+        <v>4.7702321953248202E-2</v>
       </c>
       <c r="K70" cm="1">
         <f t="array" ref="K70">_xll.FI.CURVE.FORWARD($I$2,I70)</f>
-        <v>4.8547432898258212E-2</v>
+        <v>4.8539321852524846E-2</v>
       </c>
     </row>
     <row r="71" spans="9:11" x14ac:dyDescent="0.35">
@@ -5729,11 +5731,11 @@
       </c>
       <c r="J71" cm="1">
         <f t="array" ref="J71">_xll.FI.CURVE.SPOT($I$2,I71)</f>
-        <v>4.7789226102055514E-2</v>
+        <v>4.7717268380021001E-2</v>
       </c>
       <c r="K71" cm="1">
         <f t="array" ref="K71">_xll.FI.CURVE.FORWARD($I$2,I71)</f>
-        <v>4.8547432898258212E-2</v>
+        <v>4.8539321852524846E-2</v>
       </c>
     </row>
     <row r="72" spans="9:11" x14ac:dyDescent="0.35">
@@ -5742,11 +5744,11 @@
       </c>
       <c r="J72" cm="1">
         <f t="array" ref="J72">_xll.FI.CURVE.SPOT($I$2,I72)</f>
-        <v>4.7802527975673109E-2</v>
+        <v>4.7731690370766675E-2</v>
       </c>
       <c r="K72" cm="1">
         <f t="array" ref="K72">_xll.FI.CURVE.FORWARD($I$2,I72)</f>
-        <v>4.8547432898258212E-2</v>
+        <v>4.8539321852524846E-2</v>
       </c>
     </row>
     <row r="73" spans="9:11" x14ac:dyDescent="0.35">
@@ -5755,11 +5757,11 @@
       </c>
       <c r="J73" cm="1">
         <f t="array" ref="J73">_xll.FI.CURVE.SPOT($I$2,I73)</f>
-        <v>4.7815371163993543E-2</v>
+        <v>4.7745615051486646E-2</v>
       </c>
       <c r="K73" cm="1">
         <f t="array" ref="K73">_xll.FI.CURVE.FORWARD($I$2,I73)</f>
-        <v>4.8547432898258212E-2</v>
+        <v>4.8539321852524846E-2</v>
       </c>
     </row>
     <row r="74" spans="9:11" x14ac:dyDescent="0.35">
@@ -5768,11 +5770,11 @@
       </c>
       <c r="J74" cm="1">
         <f t="array" ref="J74">_xll.FI.CURVE.SPOT($I$2,I74)</f>
-        <v>4.7827778989998029E-2</v>
+        <v>4.7759067709131367E-2</v>
       </c>
       <c r="K74" cm="1">
         <f t="array" ref="K74">_xll.FI.CURVE.FORWARD($I$2,I74)</f>
-        <v>4.8547432898258212E-2</v>
+        <v>4.8539321852524846E-2</v>
       </c>
     </row>
     <row r="75" spans="9:11" x14ac:dyDescent="0.35">
@@ -5781,11 +5783,11 @@
       </c>
       <c r="J75" cm="1">
         <f t="array" ref="J75">_xll.FI.CURVE.SPOT($I$2,I75)</f>
-        <v>4.7839773221802363E-2</v>
+        <v>4.777207194485459E-2</v>
       </c>
       <c r="K75" cm="1">
         <f t="array" ref="K75">_xll.FI.CURVE.FORWARD($I$2,I75)</f>
-        <v>4.8547432898258212E-2</v>
+        <v>4.8539321852524846E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>